<commit_message>
add solar and battery
</commit_message>
<xml_diff>
--- a/Bauteile.xlsx
+++ b/Bauteile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\LED-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C9234E-5688-4016-B1D5-C7A88D907C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D637059-7816-463C-8CE2-AA7C5E118A90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="13305" yWindow="8415" windowWidth="13365" windowHeight="8475" xr2:uid="{DE232357-304F-4507-9E84-DE7EC8554EC6}"/>
+    <workbookView xWindow="13305" yWindow="8415" windowWidth="13365" windowHeight="8475" xr2:uid="{DE232357-304F-4507-9E84-DE7EC8554EC6}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>RGB-LED</t>
   </si>
@@ -57,6 +57,78 @@
   </si>
   <si>
     <t>595-SP430G2132IPW14R</t>
+  </si>
+  <si>
+    <t>Solar-Cell</t>
+  </si>
+  <si>
+    <t>713-313070004</t>
+  </si>
+  <si>
+    <t>Kapazität</t>
+  </si>
+  <si>
+    <t>Energie</t>
+  </si>
+  <si>
+    <t>Spannung</t>
+  </si>
+  <si>
+    <t>Vas</t>
+  </si>
+  <si>
+    <t>Bei 3,3V ist das</t>
+  </si>
+  <si>
+    <t>As</t>
+  </si>
+  <si>
+    <t>und 300mA</t>
+  </si>
+  <si>
+    <t>Sekunden</t>
+  </si>
+  <si>
+    <t>Minuten</t>
+  </si>
+  <si>
+    <t>Batterie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spannung </t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>Ah</t>
+  </si>
+  <si>
+    <t>Wh</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>Ladedauer bei 0,5W (5V 100mA)</t>
+  </si>
+  <si>
+    <t>Entladedauer bei 0,99W (3,3V 300mA)</t>
+  </si>
+  <si>
+    <t>LiIo Batterie</t>
+  </si>
+  <si>
+    <t>ebay</t>
+  </si>
+  <si>
+    <t>https://www.ebay.de/itm/372645026544?_trkparms=amclksrc%3DITM%26aid%3D1110006%26algo%3DHOMESPLICE.SIM%26ao%3D1%26asc%3D240365%26meid%3Daadf40d22c504f9dbf852a7f2fa79261%26pid%3D101195%26rk%3D1%26rkt%3D12%26sd%3D115180900081%26itm%3D372645026544%26pmt%3D1%26noa%3D0%26pg%3D2047675%26algv%3DSimplAMLv9PairwiseWebMskuAspectsV202110NoVariantSeedKnnRecallV1%26brand%3DMarkenlos&amp;_trksid=p2047675.c101195.m1851&amp;amdata=cksum%3A372645026544aadf40d22c504f9dbf852a7f2fa79261%7Cenc%3AAQAHAAABMK6kjqEQMYM5Aq%252BOhcaIlwco9wYktoCXAP3D6Fo7POUdlJK1eqFqv5Y7huO6nLq7hjqYjs5sEMudJpf20WlRkR4MKodepxm8ocuu%252BsIkqh9sAsF3UwPWai9dwQfYIAw6TCsMmgwhAaTqC4u6BkSBSAMiFLslaSINciWJjezFASvA5TtOug4gthc72YlxiSC1XPcdiKmx0RTcVIUQL1oPpNYpwmqOApJ2%252B5gf5pzysfmKQyHv3IVKDzE3K7DPVIZqrI6B7h5JpG%252BekEs2UsZ9%252FvxYEyM%252FHmk7zrmryXIZPoEeVYMIRHGb7YF936l8pKcSQZftEUr5zxWM5p73I6U2MjCpI90CA52Lmw0nBtwZcPykpfM3qecXFTcVVLF6yUs3h7eM6PTHmnJd%252BaTnL0VSq04%253D%7Campid%3APL_CLK%7Cclp%3A2047675</t>
+  </si>
+  <si>
+    <t>Batteriehalter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">534-1028 </t>
   </si>
 </sst>
 </file>
@@ -408,13 +480,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{896AECD2-E8AF-47A6-8F05-A3BAA5748B87}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -474,9 +550,187 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>5.86</v>
+      </c>
       <c r="G4">
-        <f>SUM(G1:G3)</f>
-        <v>11.872</v>
+        <f>D4</f>
+        <v>5.86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5">
+        <v>5.99</v>
+      </c>
+      <c r="G5">
+        <f>D5</f>
+        <v>5.99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6">
+        <v>1.98</v>
+      </c>
+      <c r="G6">
+        <f>D6</f>
+        <v>1.98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <f>SUM(G1:G6)</f>
+        <v>25.702000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <f>0.5*B10*(B11*B11)</f>
+        <v>544.49999999999989</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <f>B12/3.3</f>
+        <v>164.99999999999997</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <f>B14/0.3</f>
+        <v>549.99999999999989</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <f>B15/60</f>
+        <v>9.1666666666666643</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>3.7</v>
+      </c>
+      <c r="C20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21">
+        <v>1.5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22">
+        <f>B20*B21</f>
+        <v>5.5500000000000007</v>
+      </c>
+      <c r="C22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23">
+        <f>B22/0.5</f>
+        <v>11.100000000000001</v>
+      </c>
+      <c r="C23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24">
+        <f>B22/(3.3*0.3)</f>
+        <v>5.6060606060606073</v>
+      </c>
+      <c r="C24" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>